<commit_message>
Troca de ehrrunner pra br-ipes
</commit_message>
<xml_diff>
--- a/output/CodeSystem-EHRDocumentTypeCodeSystem.xlsx
+++ b/output/CodeSystem-EHRDocumentTypeCodeSystem.xlsx
@@ -25,7 +25,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://ehrrunner.com/fhir/CodeSystem/EHRDocumentType</t>
+    <t>http://br-ipes.com/fhir/CodeSystem/EHRDocumentType</t>
   </si>
   <si>
     <t>Version</t>
@@ -97,7 +97,7 @@
     <t>Value Set (all codes)</t>
   </si>
   <si>
-    <t>http://ehrrunner.com/fhir/ValueSet/EHRDocumentType</t>
+    <t>http://br-ipes.com/fhir/ValueSet/EHRDocumentType</t>
   </si>
   <si>
     <t>Hierarchy</t>

</xml_diff>